<commit_message>
publish to staging - wide tables
</commit_message>
<xml_diff>
--- a/master_data/CL_SERIES.xlsx
+++ b/master_data/CL_SERIES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\ARCGIS HUBS\gender_data_portal\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4455AF5F-125E-4FEA-8812-022D569CA310}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75CF874-5CE0-4469-8963-8FA63F97DCBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE7C0272-EBF5-4B5F-81CF-57D56F39C38E}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="487">
   <si>
     <t>SORT_ORDER</t>
   </si>
@@ -1552,13 +1552,43 @@
   </si>
   <si>
     <t>Existence of law on gender statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">economy, work, </t>
+  </si>
+  <si>
+    <t>economy, employment, poverty</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>legal frameworks</t>
+  </si>
+  <si>
+    <t>legal frameworks, violence against women</t>
+  </si>
+  <si>
+    <t>legal frameworks, economy, employment</t>
+  </si>
+  <si>
+    <t>legal frameworks, family</t>
+  </si>
+  <si>
+    <t>legal frameworks, marriage</t>
+  </si>
+  <si>
+    <t>health, power</t>
+  </si>
+  <si>
+    <t>legislative, government</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -1572,6 +1602,11 @@
       <strike/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="MS Sans Serif"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="MS Sans Serif"/>
     </font>
   </fonts>
@@ -1622,7 +1657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1692,6 +1727,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2170,13 +2208,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0346C988-55B6-451E-A6D4-863A00C151F9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="K109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L116" sqref="L116"/>
+      <selection pane="bottomRight" activeCell="L124" sqref="L124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="12.75"/>
@@ -2617,7 +2656,7 @@
       <c r="M11" s="10"/>
       <c r="N11" s="19"/>
     </row>
-    <row r="12" spans="1:14" ht="25.5">
+    <row r="12" spans="1:14" ht="25.5" hidden="1">
       <c r="A12" s="10">
         <v>1100</v>
       </c>
@@ -2643,7 +2682,9 @@
       <c r="K12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="15"/>
+      <c r="L12" s="15" t="s">
+        <v>477</v>
+      </c>
       <c r="M12" s="10"/>
       <c r="N12" s="16">
         <v>79</v>
@@ -2801,7 +2842,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="25.5">
+    <row r="17" spans="1:14" ht="25.5" hidden="1">
       <c r="A17" s="10">
         <v>1600</v>
       </c>
@@ -2981,7 +3022,9 @@
       <c r="K21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L21" s="15"/>
+      <c r="L21" s="24" t="s">
+        <v>92</v>
+      </c>
       <c r="M21" s="10"/>
       <c r="N21" s="16">
         <v>81</v>
@@ -3017,7 +3060,9 @@
       <c r="K22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="15"/>
+      <c r="L22" s="24" t="s">
+        <v>66</v>
+      </c>
       <c r="M22" s="10"/>
       <c r="N22" s="16">
         <v>82</v>
@@ -3051,7 +3096,9 @@
       <c r="K23" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="15"/>
+      <c r="L23" s="24" t="s">
+        <v>66</v>
+      </c>
       <c r="M23" s="10"/>
       <c r="N23" s="16"/>
     </row>
@@ -3123,7 +3170,9 @@
       <c r="K25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="15"/>
+      <c r="L25" s="24" t="s">
+        <v>66</v>
+      </c>
       <c r="M25" s="10"/>
       <c r="N25" s="19"/>
     </row>
@@ -3157,11 +3206,13 @@
       <c r="K26" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="15"/>
+      <c r="L26" s="24" t="s">
+        <v>66</v>
+      </c>
       <c r="M26" s="10"/>
       <c r="N26" s="19"/>
     </row>
-    <row r="27" spans="1:14" ht="51">
+    <row r="27" spans="1:14" ht="51" hidden="1">
       <c r="A27" s="10">
         <v>2600</v>
       </c>
@@ -3225,11 +3276,13 @@
       <c r="K28" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="15"/>
+      <c r="L28" s="24" t="s">
+        <v>478</v>
+      </c>
       <c r="M28" s="10"/>
       <c r="N28" s="19"/>
     </row>
-    <row r="29" spans="1:14" ht="25.5">
+    <row r="29" spans="1:14" ht="25.5" hidden="1">
       <c r="A29" s="10">
         <v>2800</v>
       </c>
@@ -3335,7 +3388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="38.25">
+    <row r="32" spans="1:14" ht="38.25" hidden="1">
       <c r="A32" s="10">
         <v>3100</v>
       </c>
@@ -3655,7 +3708,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="38.25">
+    <row r="41" spans="1:14" ht="25.5">
       <c r="A41" s="10">
         <v>3200</v>
       </c>
@@ -3685,7 +3738,9 @@
       <c r="K41" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L41" s="15"/>
+      <c r="L41" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M41" s="10"/>
       <c r="N41" s="19"/>
     </row>
@@ -3719,11 +3774,13 @@
       <c r="K42" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L42" s="15"/>
+      <c r="L42" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M42" s="10"/>
       <c r="N42" s="16"/>
     </row>
-    <row r="43" spans="1:14" ht="25.5">
+    <row r="43" spans="1:14" ht="25.5" hidden="1">
       <c r="A43" s="10">
         <v>3300</v>
       </c>
@@ -3785,7 +3842,9 @@
       <c r="K44" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L44" s="15"/>
+      <c r="L44" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M44" s="10"/>
       <c r="N44" s="16">
         <v>15</v>
@@ -3821,13 +3880,15 @@
       <c r="K45" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L45" s="15"/>
+      <c r="L45" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M45" s="10"/>
       <c r="N45" s="16">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="25.5">
+    <row r="46" spans="1:14" ht="25.5" hidden="1">
       <c r="A46" s="10">
         <v>3700</v>
       </c>
@@ -3861,7 +3922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="25.5">
+    <row r="47" spans="1:14" ht="25.5" hidden="1">
       <c r="A47" s="10">
         <v>3800</v>
       </c>
@@ -3895,7 +3956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="25.5">
+    <row r="48" spans="1:14" ht="25.5" hidden="1">
       <c r="A48" s="10">
         <v>3900</v>
       </c>
@@ -3929,7 +3990,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="25.5">
+    <row r="49" spans="1:14" ht="25.5" hidden="1">
       <c r="A49" s="10">
         <v>4000</v>
       </c>
@@ -3961,7 +4022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="38.25">
+    <row r="50" spans="1:14" ht="38.25" hidden="1">
       <c r="A50" s="10">
         <v>4100</v>
       </c>
@@ -3995,7 +4056,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="25.5">
+    <row r="51" spans="1:14" ht="25.5" hidden="1">
       <c r="A51" s="10">
         <v>4200</v>
       </c>
@@ -4057,11 +4118,13 @@
       <c r="K52" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L52" s="15"/>
+      <c r="L52" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M52" s="10"/>
       <c r="N52" s="19"/>
     </row>
-    <row r="53" spans="1:14" ht="25.5">
+    <row r="53" spans="1:14" ht="25.5" hidden="1">
       <c r="A53" s="10">
         <v>4400</v>
       </c>
@@ -4125,11 +4188,13 @@
       <c r="K54" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L54" s="15"/>
+      <c r="L54" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M54" s="10"/>
       <c r="N54" s="19"/>
     </row>
-    <row r="55" spans="1:14" ht="25.5">
+    <row r="55" spans="1:14" ht="25.5" hidden="1">
       <c r="A55" s="10">
         <v>4600</v>
       </c>
@@ -4193,7 +4258,9 @@
       <c r="K56" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L56" s="15"/>
+      <c r="L56" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M56" s="10"/>
       <c r="N56" s="16"/>
     </row>
@@ -4303,11 +4370,13 @@
       <c r="K59" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="L59" s="15"/>
+      <c r="L59" s="24" t="s">
+        <v>479</v>
+      </c>
       <c r="M59" s="10"/>
       <c r="N59" s="19"/>
     </row>
-    <row r="60" spans="1:14" ht="38.25">
+    <row r="60" spans="1:14" ht="38.25" hidden="1">
       <c r="A60" s="10">
         <v>5100</v>
       </c>
@@ -4709,7 +4778,9 @@
       <c r="K70" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="L70" s="15"/>
+      <c r="L70" s="24" t="s">
+        <v>268</v>
+      </c>
       <c r="M70" s="10"/>
       <c r="N70" s="16">
         <v>28</v>
@@ -4743,7 +4814,9 @@
       <c r="K71" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="L71" s="15"/>
+      <c r="L71" s="24" t="s">
+        <v>268</v>
+      </c>
       <c r="M71" s="10"/>
       <c r="N71" s="16">
         <v>29</v>
@@ -4779,7 +4852,9 @@
       <c r="K72" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="L72" s="15"/>
+      <c r="L72" s="24" t="s">
+        <v>268</v>
+      </c>
       <c r="M72" s="10"/>
       <c r="N72" s="16">
         <v>30</v>
@@ -5267,7 +5342,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" hidden="1">
       <c r="A86" s="10">
         <v>9900</v>
       </c>
@@ -5299,7 +5374,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" hidden="1">
       <c r="A87" s="10">
         <v>10000</v>
       </c>
@@ -5331,7 +5406,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" hidden="1">
       <c r="A88" s="10">
         <v>10100</v>
       </c>
@@ -5363,7 +5438,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="25.5">
+    <row r="89" spans="1:14" ht="25.5" hidden="1">
       <c r="A89" s="10">
         <v>10200</v>
       </c>
@@ -5395,7 +5470,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="25.5">
+    <row r="90" spans="1:14" ht="25.5" hidden="1">
       <c r="A90" s="10">
         <v>10300</v>
       </c>
@@ -5427,7 +5502,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="25.5">
+    <row r="91" spans="1:14" ht="25.5" hidden="1">
       <c r="A91" s="10">
         <v>10400</v>
       </c>
@@ -5459,7 +5534,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="25.5">
+    <row r="92" spans="1:14" ht="25.5" hidden="1">
       <c r="A92" s="10">
         <v>10500</v>
       </c>
@@ -5491,7 +5566,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="25.5">
+    <row r="93" spans="1:14" ht="25.5" hidden="1">
       <c r="A93" s="10">
         <v>10600</v>
       </c>
@@ -5523,7 +5598,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="25.5">
+    <row r="94" spans="1:14" ht="25.5" hidden="1">
       <c r="A94" s="10">
         <v>10700</v>
       </c>
@@ -5555,7 +5630,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="25.5">
+    <row r="95" spans="1:14" ht="25.5" hidden="1">
       <c r="A95" s="10">
         <v>10800</v>
       </c>
@@ -5617,7 +5692,9 @@
       <c r="K96" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L96" s="15"/>
+      <c r="L96" s="15" t="s">
+        <v>480</v>
+      </c>
       <c r="M96" s="10"/>
       <c r="N96" s="19"/>
     </row>
@@ -5651,7 +5728,9 @@
       <c r="K97" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L97" s="15"/>
+      <c r="L97" s="15" t="s">
+        <v>481</v>
+      </c>
       <c r="M97" s="10"/>
       <c r="N97" s="19"/>
     </row>
@@ -5685,7 +5764,9 @@
       <c r="K98" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L98" s="15"/>
+      <c r="L98" s="15" t="s">
+        <v>482</v>
+      </c>
       <c r="M98" s="10"/>
       <c r="N98" s="19"/>
     </row>
@@ -5719,11 +5800,13 @@
       <c r="K99" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L99" s="15"/>
+      <c r="L99" s="15" t="s">
+        <v>483</v>
+      </c>
       <c r="M99" s="10"/>
       <c r="N99" s="19"/>
     </row>
-    <row r="100" spans="1:14" s="9" customFormat="1">
+    <row r="100" spans="1:14" s="9" customFormat="1" hidden="1">
       <c r="A100" s="10">
         <v>11300</v>
       </c>
@@ -5757,7 +5840,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" ht="38.25">
       <c r="A101" s="10">
         <v>11400</v>
       </c>
@@ -5785,13 +5868,15 @@
       <c r="K101" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L101" s="15"/>
+      <c r="L101" s="15" t="s">
+        <v>481</v>
+      </c>
       <c r="M101" s="10"/>
       <c r="N101" s="13">
         <v>92</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" ht="38.25">
       <c r="A102" s="10">
         <v>11500</v>
       </c>
@@ -5819,13 +5904,15 @@
       <c r="K102" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L102" s="15"/>
+      <c r="L102" s="15" t="s">
+        <v>481</v>
+      </c>
       <c r="M102" s="10"/>
       <c r="N102" s="16">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" ht="38.25">
       <c r="A103" s="10">
         <v>11600</v>
       </c>
@@ -5853,13 +5940,15 @@
       <c r="K103" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L103" s="15"/>
+      <c r="L103" s="15" t="s">
+        <v>481</v>
+      </c>
       <c r="M103" s="10"/>
       <c r="N103" s="16">
         <v>94</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="25.5">
+    <row r="104" spans="1:14" ht="25.5" hidden="1">
       <c r="A104" s="10">
         <v>11700</v>
       </c>
@@ -5967,7 +6056,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" hidden="1">
       <c r="A107" s="10">
         <v>12000</v>
       </c>
@@ -6029,7 +6118,9 @@
       <c r="K108" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L108" s="15"/>
+      <c r="L108" s="15" t="s">
+        <v>484</v>
+      </c>
       <c r="M108" s="10"/>
       <c r="N108" s="16">
         <v>97</v>
@@ -6063,7 +6154,9 @@
       <c r="K109" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L109" s="15"/>
+      <c r="L109" s="15" t="s">
+        <v>484</v>
+      </c>
       <c r="M109" s="10"/>
       <c r="N109" s="16">
         <v>98</v>
@@ -6361,7 +6454,9 @@
       <c r="K117" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="L117" s="15"/>
+      <c r="L117" s="15" t="s">
+        <v>485</v>
+      </c>
       <c r="M117" s="10"/>
       <c r="N117" s="19"/>
     </row>
@@ -6395,7 +6490,9 @@
       <c r="K118" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="L118" s="15"/>
+      <c r="L118" s="15" t="s">
+        <v>485</v>
+      </c>
       <c r="M118" s="10"/>
       <c r="N118" s="19"/>
     </row>
@@ -6429,7 +6526,9 @@
       <c r="K119" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="L119" s="15"/>
+      <c r="L119" s="15" t="s">
+        <v>485</v>
+      </c>
       <c r="M119" s="10"/>
       <c r="N119" s="19"/>
     </row>
@@ -6463,7 +6562,9 @@
       <c r="K120" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="L120" s="15"/>
+      <c r="L120" s="15" t="s">
+        <v>485</v>
+      </c>
       <c r="M120" s="10"/>
       <c r="N120" s="19"/>
     </row>
@@ -6567,14 +6668,22 @@
       <c r="K123" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="L123" s="15"/>
+      <c r="L123" s="15" t="s">
+        <v>486</v>
+      </c>
       <c r="M123" s="10"/>
       <c r="N123" s="16">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N123" xr:uid="{8C25E5C3-329E-4AC8-892C-52C8A6172AEC}"/>
+  <autoFilter ref="A1:N123" xr:uid="{8C25E5C3-329E-4AC8-892C-52C8A6172AEC}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">

</xml_diff>